<commit_message>
storage heating and different HTF util part1
</commit_message>
<xml_diff>
--- a/reskit/csp/data/CSP_database.xlsx
+++ b/reskit/csp/data/CSP_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\reskit\reskit\solar\workflows\CSP_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\reskit\reskit\csp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86065ABD-24FF-46E3-9C4F-548D1948620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0D7C61-BA7A-4769-A068-088ABDDD99E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24468" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>David Franzmann</author>
+  </authors>
+  <commentList>
+    <comment ref="Q30" authorId="0" shapeId="0" xr:uid="{244D8B4F-00AE-4EBC-AF64-68C8D4475EAD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Franzmann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+before:-1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S30" authorId="0" shapeId="0" xr:uid="{559462A3-5EB8-4F02-BA8C-5E1E04C26071}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Franzmann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+before:-1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="137">
   <si>
     <t>Parameter</t>
   </si>
@@ -430,13 +488,28 @@
   </si>
   <si>
     <t>Dataset_Heliosol_2050</t>
+  </si>
+  <si>
+    <t>eta_other</t>
+  </si>
+  <si>
+    <t>Dataset_SolarSalt_2030_validation3</t>
+  </si>
+  <si>
+    <t>Dataset_Therminol_2015</t>
+  </si>
+  <si>
+    <t>Therminol-VP1</t>
+  </si>
+  <si>
+    <t>Dataset_Therminol_2030</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +543,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -510,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -529,6 +620,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -842,17 +935,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
-  <dimension ref="A1:AA47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
+  <dimension ref="A1:AD48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="V27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="U15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z39" sqref="Z39"/>
+      <selection pane="bottomRight" activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
@@ -861,13 +954,14 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="27.5703125" customWidth="1"/>
-    <col min="19" max="19" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="26" width="27.5703125" customWidth="1"/>
-    <col min="27" max="27" width="59.7109375" customWidth="1"/>
+    <col min="14" max="16" width="27.5703125" hidden="1" customWidth="1"/>
+    <col min="17" max="19" width="27.5703125" customWidth="1"/>
+    <col min="20" max="20" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="29" width="27.5703125" customWidth="1"/>
+    <col min="30" max="30" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -923,34 +1017,43 @@
         <v>112</v>
       </c>
       <c r="S1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1003,31 +1106,40 @@
         <v>101</v>
       </c>
       <c r="S2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="15" t="s">
         <v>101</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="U2" s="15" t="s">
         <v>80</v>
       </c>
       <c r="V2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="X2" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="Y2" s="15" t="s">
         <v>80</v>
       </c>
       <c r="Z2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="15" t="s">
         <v>101</v>
       </c>
+      <c r="AB2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1083,10 +1195,10 @@
         <v>40</v>
       </c>
       <c r="S3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>110</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="U3" s="13" t="s">
         <v>18</v>
@@ -1106,11 +1218,20 @@
       <c r="Z3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1189,11 +1310,20 @@
       <c r="Z4" s="16">
         <v>8.7266462599716496E-5</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="AB4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="AC4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="AD4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1272,11 +1402,20 @@
       <c r="Z5" s="16">
         <v>3.1070976818244299E-5</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="AB5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="AC5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="AD5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1355,11 +1494,20 @@
       <c r="Z6" s="15">
         <v>0</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1417,8 +1565,8 @@
       <c r="S7" s="13">
         <v>0.92688000000000004</v>
       </c>
-      <c r="T7" s="15">
-        <v>0.82699999999999996</v>
+      <c r="T7" s="13">
+        <v>0.92688000000000004</v>
       </c>
       <c r="U7" s="15">
         <v>0.82699999999999996</v>
@@ -1438,11 +1586,20 @@
       <c r="Z7" s="15">
         <v>0.82699999999999996</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" s="15">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AB7" s="15">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AC7" s="15">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AD7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1492,8 +1649,17 @@
       <c r="Z8" s="15">
         <v>-1</v>
       </c>
+      <c r="AA8" s="15">
+        <v>-1</v>
+      </c>
+      <c r="AB8" s="15">
+        <v>-1</v>
+      </c>
+      <c r="AC8" s="15">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1572,11 +1738,20 @@
       <c r="Z9" s="15">
         <v>16</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="15">
+        <v>16</v>
+      </c>
+      <c r="AB9" s="15">
+        <v>16</v>
+      </c>
+      <c r="AC9" s="15">
+        <v>16</v>
+      </c>
+      <c r="AD9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1655,11 +1830,20 @@
       <c r="Z10" s="15">
         <v>0</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1715,34 +1899,43 @@
         <v>4.4701935910452802E-2</v>
       </c>
       <c r="S11" s="15">
+        <v>4.4701935910452829E-2</v>
+      </c>
+      <c r="T11" s="15">
         <v>4.4701935910452802E-2</v>
-      </c>
-      <c r="T11" s="15">
-        <v>4.4701935910452829E-2</v>
       </c>
       <c r="U11" s="15">
         <v>4.4701935910452829E-2</v>
       </c>
       <c r="V11" s="15">
+        <v>4.4701935910452829E-2</v>
+      </c>
+      <c r="W11" s="15">
         <v>4.4701935910452802E-2</v>
       </c>
-      <c r="W11" s="15">
+      <c r="X11" s="15">
         <v>4.4701935910452829E-2</v>
-      </c>
-      <c r="X11" s="15">
-        <v>4.4701935910452802E-2</v>
       </c>
       <c r="Y11" s="15">
         <v>4.4701935910452829E-2</v>
       </c>
       <c r="Z11" s="15">
+        <v>4.4701935910452829E-2</v>
+      </c>
+      <c r="AA11" s="15">
         <v>4.4701935910452802E-2</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" s="15">
+        <v>4.4701935910452829E-2</v>
+      </c>
+      <c r="AC11" s="15">
+        <v>4.4701935910452802E-2</v>
+      </c>
+      <c r="AD11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1821,11 +2014,20 @@
       <c r="Z12" s="15">
         <v>-2.9278818932777496E-4</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="AB12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="AC12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="AD12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1904,11 +2106,20 @@
       <c r="Z13" s="15">
         <v>1.2085236947426394E-6</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="AB13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="AC13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="AD13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1987,11 +2198,20 @@
       <c r="Z14" s="15">
         <v>-4.6531969642924003E-10</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="AB14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="AC14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="AD14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2068,8 +2288,17 @@
       <c r="Z15" s="15" t="s">
         <v>99</v>
       </c>
+      <c r="AA15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC15" s="15" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -2146,8 +2375,17 @@
       <c r="Z16" s="15">
         <v>0.38</v>
       </c>
+      <c r="AA16" s="15">
+        <v>0.38</v>
+      </c>
+      <c r="AB16" s="15">
+        <v>0.38</v>
+      </c>
+      <c r="AC16" s="15">
+        <v>0.38</v>
+      </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -2224,8 +2462,17 @@
       <c r="Z17" s="15">
         <v>0.3</v>
       </c>
+      <c r="AA17" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="AB17" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="AC17" s="15">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2305,8 +2552,17 @@
       <c r="Z18" s="10">
         <v>-1</v>
       </c>
+      <c r="AA18" s="10">
+        <v>-1</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>-1</v>
+      </c>
+      <c r="AC18" s="10">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2385,99 +2641,114 @@
       <c r="Z19" s="15">
         <v>0.96</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AA19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="AB19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="AC19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="AD19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0.108</v>
-      </c>
-      <c r="H20">
-        <v>0.108</v>
-      </c>
-      <c r="I20">
-        <v>0.108</v>
-      </c>
-      <c r="J20">
-        <v>0.108</v>
-      </c>
-      <c r="K20">
-        <v>0.108</v>
-      </c>
-      <c r="L20">
-        <v>0.108</v>
-      </c>
-      <c r="M20">
-        <v>0.108</v>
-      </c>
-      <c r="N20">
-        <v>0.108</v>
-      </c>
-      <c r="O20">
-        <v>0.108</v>
-      </c>
-      <c r="P20">
-        <v>0.108</v>
-      </c>
-      <c r="Q20">
-        <v>0.108</v>
-      </c>
-      <c r="R20">
-        <v>0.108</v>
-      </c>
-      <c r="S20">
-        <v>0.108</v>
-      </c>
-      <c r="T20">
-        <v>0.108</v>
-      </c>
-      <c r="U20">
-        <v>0.108</v>
-      </c>
-      <c r="V20">
-        <v>0.108</v>
-      </c>
-      <c r="W20">
-        <v>0.108</v>
-      </c>
-      <c r="X20">
-        <v>0.108</v>
-      </c>
-      <c r="Y20">
-        <v>0.108</v>
-      </c>
-      <c r="Z20">
-        <v>0.108</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>88</v>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10">
+        <v>1</v>
+      </c>
+      <c r="K20" s="10">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
+        <v>1</v>
+      </c>
+      <c r="N20" s="10">
+        <v>1</v>
+      </c>
+      <c r="O20" s="10">
+        <v>1</v>
+      </c>
+      <c r="P20" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>1</v>
+      </c>
+      <c r="R20" s="15">
+        <v>1</v>
+      </c>
+      <c r="S20" s="15">
+        <v>1</v>
+      </c>
+      <c r="T20" s="15">
+        <v>1</v>
+      </c>
+      <c r="U20" s="15">
+        <v>1</v>
+      </c>
+      <c r="V20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="W20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="X20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="Z20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="AA20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="AB20" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="AC20" s="15">
+        <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>33</v>
@@ -2485,245 +2756,272 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="16">
-        <v>0</v>
-      </c>
-      <c r="R21" s="16">
-        <v>0</v>
-      </c>
-      <c r="S21" s="16">
-        <v>0</v>
-      </c>
-      <c r="T21" s="16">
-        <v>0</v>
-      </c>
-      <c r="U21" s="16">
-        <v>0</v>
-      </c>
-      <c r="V21" s="16">
-        <v>0</v>
-      </c>
-      <c r="W21" s="16">
-        <v>0</v>
-      </c>
-      <c r="X21" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA21" t="s">
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.108</v>
+      </c>
+      <c r="H21">
+        <v>0.108</v>
+      </c>
+      <c r="I21">
+        <v>0.108</v>
+      </c>
+      <c r="J21">
+        <v>0.108</v>
+      </c>
+      <c r="K21">
+        <v>0.108</v>
+      </c>
+      <c r="L21">
+        <v>0.108</v>
+      </c>
+      <c r="M21">
+        <v>0.108</v>
+      </c>
+      <c r="N21">
+        <v>0.108</v>
+      </c>
+      <c r="O21">
+        <v>0.108</v>
+      </c>
+      <c r="P21">
+        <v>0.108</v>
+      </c>
+      <c r="Q21">
+        <v>0.108</v>
+      </c>
+      <c r="R21">
+        <v>0.108</v>
+      </c>
+      <c r="S21">
+        <v>0.108</v>
+      </c>
+      <c r="T21">
+        <v>0.108</v>
+      </c>
+      <c r="U21">
+        <v>0.108</v>
+      </c>
+      <c r="V21">
+        <v>0.108</v>
+      </c>
+      <c r="W21">
+        <v>0.108</v>
+      </c>
+      <c r="X21">
+        <v>0.108</v>
+      </c>
+      <c r="Y21">
+        <v>0.108</v>
+      </c>
+      <c r="Z21">
+        <v>0.108</v>
+      </c>
+      <c r="AA21">
+        <v>0.108</v>
+      </c>
+      <c r="AB21">
+        <v>0.108</v>
+      </c>
+      <c r="AC21">
+        <v>0.108</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>0</v>
+      </c>
+      <c r="R22" s="16">
+        <v>0</v>
+      </c>
+      <c r="S22" s="16">
+        <v>0</v>
+      </c>
+      <c r="T22" s="16">
+        <v>0</v>
+      </c>
+      <c r="U22" s="16">
+        <v>0</v>
+      </c>
+      <c r="V22" s="16">
+        <v>0</v>
+      </c>
+      <c r="W22" s="16">
+        <v>0</v>
+      </c>
+      <c r="X22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:30">
+      <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22">
-        <v>600</v>
-      </c>
-      <c r="E22">
-        <v>600</v>
-      </c>
-      <c r="F22">
-        <v>600</v>
-      </c>
-      <c r="G22">
-        <v>600</v>
-      </c>
-      <c r="H22">
-        <v>600</v>
-      </c>
-      <c r="I22">
-        <v>600</v>
-      </c>
-      <c r="J22">
-        <v>600</v>
-      </c>
-      <c r="K22">
-        <v>600</v>
-      </c>
-      <c r="L22">
-        <v>600</v>
-      </c>
-      <c r="M22">
-        <v>600</v>
-      </c>
-      <c r="N22">
-        <v>600</v>
-      </c>
-      <c r="O22">
-        <v>900</v>
-      </c>
-      <c r="P22">
-        <v>900</v>
-      </c>
-      <c r="Q22" s="15">
-        <v>830</v>
-      </c>
-      <c r="R22" s="15">
-        <v>830</v>
-      </c>
-      <c r="S22" s="15">
-        <v>830</v>
-      </c>
-      <c r="T22" s="15">
-        <v>830</v>
-      </c>
-      <c r="U22" s="15">
-        <v>830</v>
-      </c>
-      <c r="V22" s="15">
-        <v>830</v>
-      </c>
-      <c r="W22" s="15">
-        <v>830</v>
-      </c>
-      <c r="X22" s="15">
-        <v>830</v>
-      </c>
-      <c r="Y22" s="15">
-        <v>830</v>
-      </c>
-      <c r="Z22" s="15">
-        <v>830</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="E23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="F23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="G23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="H23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="I23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="J23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="K23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="L23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="M23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="N23">
-        <v>5.4999999999999997E-3</v>
+        <v>600</v>
       </c>
       <c r="O23">
-        <v>5.4999999999999997E-3</v>
+        <v>900</v>
       </c>
       <c r="P23">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="R23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="S23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="T23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="U23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="V23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="W23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="X23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="AA23" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>830</v>
+      </c>
+      <c r="R23" s="15">
+        <v>830</v>
+      </c>
+      <c r="S23" s="15">
+        <v>830</v>
+      </c>
+      <c r="T23" s="15">
+        <v>830</v>
+      </c>
+      <c r="U23" s="15">
+        <v>830</v>
+      </c>
+      <c r="V23" s="15">
+        <v>830</v>
+      </c>
+      <c r="W23" s="15">
+        <v>830</v>
+      </c>
+      <c r="X23" s="15">
+        <v>830</v>
+      </c>
+      <c r="Y23" s="15">
+        <v>830</v>
+      </c>
+      <c r="Z23" s="15">
+        <v>830</v>
+      </c>
+      <c r="AA23" s="15">
+        <v>830</v>
+      </c>
+      <c r="AB23" s="15">
+        <v>830</v>
+      </c>
+      <c r="AC23" s="15">
+        <v>830</v>
+      </c>
+      <c r="AD23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>44</v>
@@ -2732,81 +3030,90 @@
         <v>74</v>
       </c>
       <c r="D24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="E24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="G24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="H24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="I24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="J24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="K24">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="L24" s="7">
-        <v>1.6E-2</v>
-      </c>
-      <c r="M24" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="N24" s="9">
-        <v>1.6E-2</v>
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="L24">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="M24">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="N24">
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="O24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="P24">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="Q24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="R24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="S24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="T24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="U24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="V24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="W24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="X24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="Y24" s="7">
-        <v>2.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="Z24" s="7">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="AA24" t="s">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AA24" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AC24" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AD24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>44</v>
@@ -2815,81 +3122,90 @@
         <v>74</v>
       </c>
       <c r="D25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="F25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="G25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="H25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="I25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="J25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="K25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="L25" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M25" s="7">
-        <v>1.15E-2</v>
-      </c>
-      <c r="N25" s="12">
-        <v>1.15E-2</v>
+        <v>1.6E-2</v>
+      </c>
+      <c r="M25" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1.6E-2</v>
       </c>
       <c r="O25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="P25">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="Q25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="R25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="S25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="T25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="U25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="V25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="W25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="X25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="Y25" s="7">
-        <v>0.05</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="Z25" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="AA25" t="s">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AA25" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AB25" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AC25" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AD25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>44</v>
@@ -2898,81 +3214,90 @@
         <v>74</v>
       </c>
       <c r="D26">
+        <v>0.05</v>
+      </c>
+      <c r="E26">
+        <v>0.05</v>
+      </c>
+      <c r="F26">
+        <v>0.05</v>
+      </c>
+      <c r="G26">
+        <v>0.05</v>
+      </c>
+      <c r="H26">
+        <v>0.05</v>
+      </c>
+      <c r="I26">
+        <v>0.05</v>
+      </c>
+      <c r="J26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
+        <v>0.05</v>
+      </c>
+      <c r="L26" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="J26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="N26">
-        <v>3.0000000000000001E-3</v>
+      <c r="M26" s="7">
+        <v>1.15E-2</v>
+      </c>
+      <c r="N26" s="12">
+        <v>1.15E-2</v>
       </c>
       <c r="O26">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="P26">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="Q26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="R26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="S26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="T26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="U26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="V26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="W26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="X26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="Y26" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="Z26" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AA26" t="s">
+        <v>0.05</v>
+      </c>
+      <c r="AA26" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AC26" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AD26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>44</v>
@@ -2981,390 +3306,425 @@
         <v>74</v>
       </c>
       <c r="D27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="T27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="U27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="W27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="X27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AA27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28">
         <v>1.9E-2</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>1.9E-2</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>1.9E-2</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>1.9E-2</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>1.9E-2</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <v>1.9E-2</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <v>1.9E-2</v>
       </c>
-      <c r="K27">
+      <c r="K28">
         <v>1.9E-2</v>
       </c>
-      <c r="L27">
+      <c r="L28">
         <v>1.9E-2</v>
       </c>
-      <c r="M27">
+      <c r="M28">
         <v>1.9E-2</v>
       </c>
-      <c r="N27">
+      <c r="N28">
         <v>1.9E-2</v>
       </c>
-      <c r="O27">
+      <c r="O28">
         <v>1.9E-2</v>
       </c>
-      <c r="P27">
+      <c r="P28">
         <v>1.9E-2</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="U27" s="7">
+      <c r="U28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="V27" s="7">
+      <c r="V28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="W27" s="7">
+      <c r="W28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="X27" s="7">
+      <c r="X28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="Y27" s="7">
+      <c r="Y28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="Z27" s="7">
+      <c r="Z28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AA28" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AD28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:30">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>1100</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E29" s="4">
         <v>1100</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F29" s="4">
         <v>1100</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G29" s="4">
         <v>1100</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H29" s="5">
         <v>3688</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I29" s="6">
         <v>3688</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J29" s="5">
         <v>1100</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K29" s="5">
         <v>3688</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L29" s="6">
         <v>3688</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M29" s="6">
         <v>3688</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N29" s="6">
         <v>3688</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O29" s="6">
         <v>3688</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P29" s="6">
         <v>3688</v>
       </c>
-      <c r="Q28" s="7">
-        <f>P28*4/3</f>
+      <c r="Q29" s="7">
         <v>4917.333333333333</v>
       </c>
-      <c r="R28" s="7">
-        <f>P28*10/14</f>
+      <c r="R29" s="7">
         <v>2634.2857142857142</v>
       </c>
-      <c r="S28" s="7">
-        <f>Q28*10/14</f>
-        <v>3512.3809523809518</v>
-      </c>
-      <c r="T28" s="7">
-        <f>S28*4/3</f>
-        <v>4683.1746031746025</v>
-      </c>
-      <c r="U28" s="7">
-        <f>T28*4/3</f>
-        <v>6244.2328042328036</v>
-      </c>
-      <c r="V28" s="7">
-        <f>S28*10/14</f>
-        <v>2508.8435374149658</v>
-      </c>
-      <c r="W28" s="7">
-        <f>V28*4/3</f>
-        <v>3345.1247165532877</v>
-      </c>
-      <c r="X28" s="7">
-        <f>U28*10/14</f>
-        <v>4460.166288737717</v>
-      </c>
-      <c r="Y28" s="7">
-        <f>X28*4/3</f>
-        <v>5946.8883849836229</v>
-      </c>
-      <c r="Z28" s="7">
-        <f>W28*10/14</f>
-        <v>2389.3747975380625</v>
-      </c>
-      <c r="AA28" t="s">
+      <c r="S29" s="7">
+        <v>6500</v>
+      </c>
+      <c r="T29" s="7">
+        <v>2634.2857142857142</v>
+      </c>
+      <c r="U29" s="7">
+        <v>4917.333333333333</v>
+      </c>
+      <c r="V29" s="7">
+        <v>6500</v>
+      </c>
+      <c r="W29" s="7">
+        <v>2634.2857142857142</v>
+      </c>
+      <c r="X29" s="19">
+        <v>3688</v>
+      </c>
+      <c r="Y29" s="19">
+        <v>3688</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>6500</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>2634.2857142857142</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>6500</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>2634.2857142857142</v>
+      </c>
+      <c r="AD29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:30">
+      <c r="A30" t="s">
         <v>116</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="7">
-        <v>-1</v>
-      </c>
-      <c r="R29" s="7">
-        <v>-1</v>
-      </c>
-      <c r="S29" s="7">
-        <v>-1</v>
-      </c>
-      <c r="T29" s="7">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="U29" s="7">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="V29" s="7">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="W29" s="7">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="X29" s="7">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="Y29" s="7">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="Z29" s="7">
-        <v>0.39100000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>114</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="18">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="R30" s="18">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="S30" s="18">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="T30" s="7">
+        <v>-1</v>
+      </c>
+      <c r="U30" s="7">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="V30" s="7">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="W30" s="7">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="X30" s="7">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="Z30" s="7">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="AA30" s="7">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="AB30" s="7">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="AC30" s="7">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.98</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>0.98</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>0.98</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>0.98</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>0.98</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <v>0.98</v>
       </c>
-      <c r="J30">
+      <c r="J31">
         <v>0.98</v>
       </c>
-      <c r="K30">
+      <c r="K31">
         <v>0.98</v>
       </c>
-      <c r="L30">
+      <c r="L31">
         <v>0.98</v>
       </c>
-      <c r="M30">
+      <c r="M31">
         <v>0.98</v>
       </c>
-      <c r="N30">
+      <c r="N31">
         <v>0.98</v>
       </c>
-      <c r="O30">
+      <c r="O31">
         <v>0.98</v>
       </c>
-      <c r="P30">
+      <c r="P31">
         <v>0.98</v>
       </c>
-      <c r="Q30">
+      <c r="Q31">
         <v>0.98</v>
       </c>
-      <c r="R30">
+      <c r="R31">
         <v>0.98</v>
       </c>
-      <c r="S30">
+      <c r="S31">
         <v>0.98</v>
       </c>
-      <c r="T30">
+      <c r="T31">
         <v>0.98</v>
       </c>
-      <c r="U30">
+      <c r="U31">
         <v>0.98</v>
       </c>
-      <c r="V30">
+      <c r="V31">
         <v>0.98</v>
       </c>
-      <c r="W30">
+      <c r="W31">
         <v>0.98</v>
       </c>
-      <c r="X30">
+      <c r="X31">
         <v>0.98</v>
       </c>
-      <c r="Y30">
+      <c r="Y31">
         <v>0.98</v>
       </c>
-      <c r="Z30">
+      <c r="Z31">
         <v>0.98</v>
       </c>
+      <c r="AA31">
+        <v>0.98</v>
+      </c>
+      <c r="AB31">
+        <v>0.98</v>
+      </c>
+      <c r="AC31">
+        <v>0.98</v>
+      </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:30">
+      <c r="A32" t="s">
         <v>13</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31">
-        <v>385</v>
-      </c>
-      <c r="E31" s="4">
-        <v>385</v>
-      </c>
-      <c r="F31" s="4">
-        <v>385</v>
-      </c>
-      <c r="G31" s="4">
-        <v>385</v>
-      </c>
-      <c r="H31" s="6">
-        <v>385</v>
-      </c>
-      <c r="I31" s="6">
-        <v>385</v>
-      </c>
-      <c r="J31" s="6">
-        <v>385</v>
-      </c>
-      <c r="K31" s="6">
-        <v>385</v>
-      </c>
-      <c r="L31" s="6">
-        <v>385</v>
-      </c>
-      <c r="M31" s="6">
-        <v>385</v>
-      </c>
-      <c r="N31" s="6">
-        <v>385</v>
-      </c>
-      <c r="O31" s="6">
-        <v>550</v>
-      </c>
-      <c r="P31" s="6">
-        <v>550</v>
-      </c>
-      <c r="Q31" s="7">
-        <v>560</v>
-      </c>
-      <c r="R31" s="15">
-        <v>405</v>
-      </c>
-      <c r="S31" s="15">
-        <v>405</v>
-      </c>
-      <c r="T31" s="7">
-        <v>560</v>
-      </c>
-      <c r="U31" s="7">
-        <v>560</v>
-      </c>
-      <c r="V31" s="15">
-        <v>405</v>
-      </c>
-      <c r="W31" s="7">
-        <v>560</v>
-      </c>
-      <c r="X31" s="15">
-        <v>405</v>
-      </c>
-      <c r="Y31" s="7">
-        <v>560</v>
-      </c>
-      <c r="Z31" s="15">
-        <v>405</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>14</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>25</v>
@@ -3373,81 +3733,90 @@
         <v>35</v>
       </c>
       <c r="D32">
-        <v>15</v>
-      </c>
-      <c r="E32" s="5">
-        <v>60</v>
+        <v>385</v>
+      </c>
+      <c r="E32" s="4">
+        <v>385</v>
       </c>
       <c r="F32" s="4">
-        <v>60</v>
+        <v>385</v>
       </c>
       <c r="G32" s="4">
-        <v>60</v>
-      </c>
-      <c r="H32" s="4">
-        <v>60</v>
-      </c>
-      <c r="I32" s="4">
-        <v>60</v>
-      </c>
-      <c r="J32" s="4">
-        <v>60</v>
-      </c>
-      <c r="K32" s="4">
-        <v>60</v>
-      </c>
-      <c r="L32" s="4">
-        <v>60</v>
-      </c>
-      <c r="M32" s="4">
-        <v>60</v>
-      </c>
-      <c r="N32" s="4">
-        <v>60</v>
-      </c>
-      <c r="O32" s="4">
-        <v>260</v>
-      </c>
-      <c r="P32" s="4">
-        <v>260</v>
+        <v>385</v>
+      </c>
+      <c r="H32" s="6">
+        <v>385</v>
+      </c>
+      <c r="I32" s="6">
+        <v>385</v>
+      </c>
+      <c r="J32" s="6">
+        <v>385</v>
+      </c>
+      <c r="K32" s="6">
+        <v>385</v>
+      </c>
+      <c r="L32" s="6">
+        <v>385</v>
+      </c>
+      <c r="M32" s="6">
+        <v>385</v>
+      </c>
+      <c r="N32" s="6">
+        <v>385</v>
+      </c>
+      <c r="O32" s="6">
+        <v>550</v>
+      </c>
+      <c r="P32" s="6">
+        <v>550</v>
       </c>
       <c r="Q32" s="7">
-        <v>260</v>
+        <v>560</v>
       </c>
       <c r="R32" s="15">
-        <v>-20</v>
-      </c>
-      <c r="S32" s="15">
-        <v>-20</v>
-      </c>
-      <c r="T32" s="7">
-        <v>260</v>
+        <v>405</v>
+      </c>
+      <c r="S32" s="7">
+        <v>560</v>
+      </c>
+      <c r="T32" s="15">
+        <v>405</v>
       </c>
       <c r="U32" s="7">
-        <v>260</v>
-      </c>
-      <c r="V32" s="15">
-        <v>-20</v>
-      </c>
-      <c r="W32" s="7">
-        <v>260</v>
-      </c>
-      <c r="X32" s="15">
-        <v>-20</v>
+        <v>560</v>
+      </c>
+      <c r="V32" s="7">
+        <v>560</v>
+      </c>
+      <c r="W32" s="15">
+        <v>405</v>
+      </c>
+      <c r="X32" s="7">
+        <v>385</v>
       </c>
       <c r="Y32" s="7">
-        <v>260</v>
-      </c>
-      <c r="Z32" s="15">
-        <v>-20</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>92</v>
+        <v>385</v>
+      </c>
+      <c r="Z32" s="7">
+        <v>560</v>
+      </c>
+      <c r="AA32" s="15">
+        <v>405</v>
+      </c>
+      <c r="AB32" s="7">
+        <v>560</v>
+      </c>
+      <c r="AC32" s="15">
+        <v>405</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>25</v>
@@ -3456,561 +3825,627 @@
         <v>35</v>
       </c>
       <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33" s="5">
+        <v>60</v>
+      </c>
+      <c r="F33" s="4">
+        <v>60</v>
+      </c>
+      <c r="G33" s="4">
+        <v>60</v>
+      </c>
+      <c r="H33" s="4">
+        <v>60</v>
+      </c>
+      <c r="I33" s="4">
+        <v>60</v>
+      </c>
+      <c r="J33" s="4">
+        <v>60</v>
+      </c>
+      <c r="K33" s="4">
+        <v>60</v>
+      </c>
+      <c r="L33" s="4">
+        <v>60</v>
+      </c>
+      <c r="M33" s="4">
+        <v>60</v>
+      </c>
+      <c r="N33" s="4">
+        <v>60</v>
+      </c>
+      <c r="O33" s="4">
+        <v>260</v>
+      </c>
+      <c r="P33" s="4">
+        <v>260</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>260</v>
+      </c>
+      <c r="R33" s="15">
+        <v>-20</v>
+      </c>
+      <c r="S33" s="7">
+        <v>260</v>
+      </c>
+      <c r="T33" s="15">
+        <v>-20</v>
+      </c>
+      <c r="U33" s="7">
+        <v>260</v>
+      </c>
+      <c r="V33" s="7">
+        <v>260</v>
+      </c>
+      <c r="W33" s="15">
+        <v>-20</v>
+      </c>
+      <c r="X33" s="7">
+        <v>60</v>
+      </c>
+      <c r="Y33" s="7">
+        <v>60</v>
+      </c>
+      <c r="Z33" s="7">
+        <v>260</v>
+      </c>
+      <c r="AA33" s="15">
+        <v>-20</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>260</v>
+      </c>
+      <c r="AC33" s="15">
+        <v>-20</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34">
         <v>295</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>295</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>295</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>295</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>295</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>295</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>295</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>295</v>
       </c>
-      <c r="L33">
+      <c r="L34">
         <v>295</v>
       </c>
-      <c r="M33">
+      <c r="M34">
         <v>295</v>
       </c>
-      <c r="N33">
+      <c r="N34">
         <v>295</v>
       </c>
-      <c r="O33" s="4">
+      <c r="O34" s="4">
         <v>295</v>
       </c>
-      <c r="P33" s="4">
+      <c r="P34" s="4">
         <v>295</v>
       </c>
-      <c r="Q33" s="7">
+      <c r="Q34" s="7">
         <v>290</v>
       </c>
-      <c r="R33" s="15">
+      <c r="R34" s="15">
         <v>290</v>
       </c>
-      <c r="S33" s="15">
+      <c r="S34" s="7">
         <v>290</v>
       </c>
-      <c r="T33" s="7">
+      <c r="T34" s="15">
         <v>290</v>
       </c>
-      <c r="U33" s="7">
+      <c r="U34" s="7">
         <v>290</v>
       </c>
-      <c r="V33" s="15">
+      <c r="V34" s="7">
         <v>290</v>
       </c>
-      <c r="W33" s="7">
+      <c r="W34" s="15">
         <v>290</v>
       </c>
-      <c r="X33" s="15">
+      <c r="X34" s="7">
         <v>290</v>
       </c>
-      <c r="Y33" s="7">
+      <c r="Y34" s="7">
         <v>290</v>
       </c>
-      <c r="Z33" s="15">
+      <c r="Z34" s="7">
         <v>290</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AA34" s="15">
+        <v>290</v>
+      </c>
+      <c r="AB34" s="7">
+        <v>290</v>
+      </c>
+      <c r="AC34" s="15">
+        <v>290</v>
+      </c>
+      <c r="AD34" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:30">
+      <c r="A35" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>40</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>40</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>40</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>40</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <v>40</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <v>40</v>
       </c>
-      <c r="J34">
+      <c r="J35">
         <v>40</v>
       </c>
-      <c r="K34">
+      <c r="K35">
         <v>40</v>
       </c>
-      <c r="L34">
+      <c r="L35">
         <v>40</v>
       </c>
-      <c r="M34">
+      <c r="M35">
         <v>40</v>
       </c>
-      <c r="N34">
+      <c r="N35">
         <v>40</v>
       </c>
-      <c r="O34">
+      <c r="O35">
         <v>40</v>
       </c>
-      <c r="P34">
+      <c r="P35">
         <v>25</v>
       </c>
-      <c r="Q34">
+      <c r="Q35">
         <v>25</v>
       </c>
-      <c r="R34">
+      <c r="R35">
         <v>25</v>
       </c>
-      <c r="S34">
+      <c r="S35">
         <v>25</v>
       </c>
-      <c r="T34">
+      <c r="T35">
         <v>25</v>
       </c>
-      <c r="U34">
+      <c r="U35">
         <v>25</v>
       </c>
-      <c r="V34">
+      <c r="V35">
         <v>25</v>
       </c>
-      <c r="W34">
+      <c r="W35">
         <v>25</v>
       </c>
-      <c r="X34">
+      <c r="X35">
         <v>25</v>
       </c>
-      <c r="Y34">
+      <c r="Y35">
         <v>25</v>
       </c>
-      <c r="Z34">
+      <c r="Z35">
         <v>25</v>
       </c>
+      <c r="AA35">
+        <v>25</v>
+      </c>
+      <c r="AB35">
+        <v>25</v>
+      </c>
+      <c r="AC35">
+        <v>25</v>
+      </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:30">
+      <c r="A36" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="E35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="F35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="G35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="H35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="I35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="J35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="K35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="L35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="M35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="N35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="O35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="P35" s="17">
-        <v>1140</v>
-      </c>
-      <c r="Q35" s="15">
-        <v>1140</v>
-      </c>
-      <c r="R35" s="15">
-        <v>1140</v>
-      </c>
-      <c r="S35" s="15">
-        <v>1140</v>
-      </c>
-      <c r="T35" s="15">
-        <v>1220</v>
-      </c>
-      <c r="U35" s="15">
-        <v>1003.2</v>
-      </c>
-      <c r="V35" s="15">
-        <v>1003.2</v>
-      </c>
-      <c r="W35" s="15">
-        <v>922.94399999999996</v>
-      </c>
-      <c r="X35" s="15">
-        <v>922.94399999999996</v>
-      </c>
-      <c r="Y35" s="15">
-        <v>882.81600000000003</v>
-      </c>
-      <c r="Z35" s="15">
-        <v>882.81600000000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="E36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="F36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="G36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="H36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="I36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="J36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="K36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="L36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="M36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="N36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="O36" s="17">
-        <v>29</v>
+        <v>1140</v>
       </c>
       <c r="P36" s="17">
-        <v>29</v>
-      </c>
-      <c r="Q36" s="7">
-        <v>29</v>
+        <v>1140</v>
+      </c>
+      <c r="Q36" s="15">
+        <v>1140</v>
       </c>
       <c r="R36" s="15">
-        <v>42</v>
+        <v>1140</v>
       </c>
       <c r="S36" s="15">
-        <v>42</v>
-      </c>
-      <c r="T36" s="7">
-        <v>42</v>
-      </c>
-      <c r="U36" s="7">
-        <v>25.52</v>
+        <v>1140</v>
+      </c>
+      <c r="T36" s="15">
+        <v>1140</v>
+      </c>
+      <c r="U36" s="15">
+        <v>1220</v>
       </c>
       <c r="V36" s="15">
-        <v>36.96</v>
-      </c>
-      <c r="W36" s="7">
-        <v>23.478400000000001</v>
+        <v>1003.2</v>
+      </c>
+      <c r="W36" s="15">
+        <v>1003.2</v>
       </c>
       <c r="X36" s="15">
-        <v>34.0032</v>
-      </c>
-      <c r="Y36" s="7">
-        <v>22.457599999999999</v>
+        <v>1056</v>
+      </c>
+      <c r="Y36" s="15">
+        <v>1003.2</v>
       </c>
       <c r="Z36" s="15">
-        <v>32.524799999999999</v>
+        <v>922.94399999999996</v>
+      </c>
+      <c r="AA36" s="15">
+        <v>922.94399999999996</v>
+      </c>
+      <c r="AB36" s="15">
+        <v>882.81600000000003</v>
+      </c>
+      <c r="AC36" s="15">
+        <v>882.81600000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="E37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="F37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="G37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="H37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="I37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="J37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="K37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="L37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="M37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="N37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="O37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="P37" s="17">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="Q37" s="7">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="R37" s="15">
-        <v>219</v>
-      </c>
-      <c r="S37" s="15">
-        <v>219</v>
-      </c>
-      <c r="T37" s="7">
-        <v>231</v>
+        <v>42</v>
+      </c>
+      <c r="S37" s="7">
+        <v>29</v>
+      </c>
+      <c r="T37" s="15">
+        <v>42</v>
       </c>
       <c r="U37" s="7">
-        <v>165.44</v>
-      </c>
-      <c r="V37" s="15">
-        <v>192.72</v>
-      </c>
-      <c r="W37" s="7">
-        <v>152.19999999999999</v>
-      </c>
-      <c r="X37" s="15">
-        <v>177.30240000000001</v>
+        <v>42</v>
+      </c>
+      <c r="V37" s="7">
+        <v>25.52</v>
+      </c>
+      <c r="W37" s="15">
+        <v>36.96</v>
+      </c>
+      <c r="X37" s="7">
+        <v>44</v>
       </c>
       <c r="Y37" s="7">
-        <v>145.5872</v>
-      </c>
-      <c r="Z37" s="15">
-        <v>169.59360000000001</v>
+        <v>36.96</v>
+      </c>
+      <c r="Z37" s="7">
+        <v>23.478400000000001</v>
+      </c>
+      <c r="AA37" s="15">
+        <v>34.0032</v>
+      </c>
+      <c r="AB37" s="7">
+        <v>22.457599999999999</v>
+      </c>
+      <c r="AC37" s="15">
+        <v>32.524799999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="E38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="F38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="G38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="H38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="I38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="J38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="K38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="L38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="M38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="N38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="O38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="P38" s="17">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="Q38" s="7">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="R38" s="15">
-        <v>1</v>
-      </c>
-      <c r="S38" s="15">
-        <v>1</v>
-      </c>
-      <c r="T38" s="7">
-        <v>1</v>
+        <v>219</v>
+      </c>
+      <c r="S38" s="7">
+        <v>188</v>
+      </c>
+      <c r="T38" s="15">
+        <v>219</v>
       </c>
       <c r="U38" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="V38" s="15">
-        <v>0.88</v>
-      </c>
-      <c r="W38" s="7">
-        <v>0.8196</v>
-      </c>
-      <c r="X38" s="15">
-        <v>0.8196</v>
+        <v>231</v>
+      </c>
+      <c r="V38" s="7">
+        <v>165.44</v>
+      </c>
+      <c r="W38" s="15">
+        <v>192.72</v>
+      </c>
+      <c r="X38" s="7">
+        <v>220</v>
       </c>
       <c r="Y38" s="7">
-        <v>0.77439999999999998</v>
-      </c>
-      <c r="Z38" s="15">
-        <v>0.77439999999999998</v>
+        <v>172.21600000000001</v>
+      </c>
+      <c r="Z38" s="7">
+        <v>152.19999999999999</v>
+      </c>
+      <c r="AA38" s="15">
+        <v>177.30240000000001</v>
+      </c>
+      <c r="AB38" s="7">
+        <v>145.5872</v>
+      </c>
+      <c r="AC38" s="15">
+        <v>169.59360000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="M39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="O39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="P39" s="17">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="Q39" s="7">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="R39" s="15">
-        <v>11</v>
-      </c>
-      <c r="S39" s="15">
-        <v>11</v>
-      </c>
-      <c r="T39" s="7">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="S39" s="7">
+        <v>1</v>
+      </c>
+      <c r="T39" s="15">
+        <v>1</v>
       </c>
       <c r="U39" s="7">
-        <v>11</v>
-      </c>
-      <c r="V39" s="15">
-        <v>11</v>
-      </c>
-      <c r="W39" s="7">
-        <v>11</v>
-      </c>
-      <c r="X39" s="15">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="V39" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="W39" s="15">
+        <v>0.88</v>
+      </c>
+      <c r="X39" s="7">
+        <v>0.88</v>
       </c>
       <c r="Y39" s="7">
-        <v>11</v>
-      </c>
-      <c r="Z39" s="15">
-        <v>11</v>
+        <v>0.88</v>
+      </c>
+      <c r="Z39" s="7">
+        <v>0.8196</v>
+      </c>
+      <c r="AA39" s="15">
+        <v>0.8196</v>
+      </c>
+      <c r="AB39" s="7">
+        <v>0.77439999999999998</v>
+      </c>
+      <c r="AC39" s="15">
+        <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>104</v>
@@ -4019,398 +4454,443 @@
         <v>105</v>
       </c>
       <c r="D40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="L40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="M40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="O40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="P40" s="17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="Q40" s="7">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="R40" s="15">
-        <v>2</v>
-      </c>
-      <c r="S40" s="15">
-        <v>2</v>
-      </c>
-      <c r="T40" s="7">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="S40" s="7">
+        <v>11</v>
+      </c>
+      <c r="T40" s="15">
+        <v>11</v>
       </c>
       <c r="U40" s="7">
-        <v>2</v>
-      </c>
-      <c r="V40" s="15">
-        <v>2</v>
-      </c>
-      <c r="W40" s="7">
-        <v>2</v>
-      </c>
-      <c r="X40" s="15">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="V40" s="7">
+        <v>11</v>
+      </c>
+      <c r="W40" s="15">
+        <v>11</v>
+      </c>
+      <c r="X40" s="7">
+        <v>15</v>
       </c>
       <c r="Y40" s="7">
-        <v>2</v>
-      </c>
-      <c r="Z40" s="15">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="Z40" s="7">
+        <v>11</v>
+      </c>
+      <c r="AA40" s="15">
+        <v>11</v>
+      </c>
+      <c r="AB40" s="7">
+        <v>11</v>
+      </c>
+      <c r="AC40" s="15">
+        <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="E41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="F41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="G41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="H41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="I41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="J41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="K41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="L41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="M41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="N41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="O41" s="17">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="P41" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="Q41" s="15">
-        <v>0.05</v>
+        <v>2</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>2</v>
       </c>
       <c r="R41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="S41" s="15">
-        <v>0.05</v>
+        <v>2</v>
+      </c>
+      <c r="S41" s="7">
+        <v>2</v>
       </c>
       <c r="T41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="U41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="V41" s="15">
-        <v>0.05</v>
+        <v>2</v>
+      </c>
+      <c r="U41" s="7">
+        <v>2</v>
+      </c>
+      <c r="V41" s="7">
+        <v>2</v>
       </c>
       <c r="W41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="X41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="Y41" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="Z41" s="15">
-        <v>0.05</v>
+        <v>2</v>
+      </c>
+      <c r="X41" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y41" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA41" s="15">
+        <v>2</v>
+      </c>
+      <c r="AB41" s="7">
+        <v>2</v>
+      </c>
+      <c r="AC41" s="15">
+        <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="E42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="F42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="H42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="I42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="J42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="K42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="L42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="M42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="N42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="O42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="P42" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="Q42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="R42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="S42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="T42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="U42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="V42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="W42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="X42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="Y42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="Z42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="AA42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="AB42" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="AC42" s="15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="17">
         <v>8</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E43" s="17">
         <v>8</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F43" s="17">
         <v>8</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G43" s="17">
         <v>8</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H43" s="17">
         <v>8</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I43" s="17">
         <v>8</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J43" s="17">
         <v>8</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K43" s="17">
         <v>8</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L43" s="17">
         <v>8</v>
       </c>
-      <c r="M42" s="17">
+      <c r="M43" s="17">
         <v>8</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N43" s="17">
         <v>8</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O43" s="17">
         <v>8</v>
       </c>
-      <c r="P42" s="17">
+      <c r="P43" s="17">
         <v>8</v>
       </c>
-      <c r="Q42" s="15">
+      <c r="Q43" s="15">
         <v>8</v>
       </c>
-      <c r="R42" s="15">
+      <c r="R43" s="15">
         <v>8</v>
       </c>
-      <c r="S42" s="15">
+      <c r="S43" s="15">
         <v>8</v>
       </c>
-      <c r="T42" s="15">
+      <c r="T43" s="15">
         <v>8</v>
       </c>
-      <c r="U42" s="15">
+      <c r="U43" s="15">
         <v>8</v>
       </c>
-      <c r="V42" s="15">
+      <c r="V43" s="15">
         <v>8</v>
       </c>
-      <c r="W42" s="15">
+      <c r="W43" s="15">
         <v>8</v>
       </c>
-      <c r="X42" s="15">
+      <c r="X43" s="15">
         <v>8</v>
       </c>
-      <c r="Y42" s="15">
+      <c r="Y43" s="15">
         <v>8</v>
       </c>
-      <c r="Z42" s="15">
+      <c r="Z43" s="15">
         <v>8</v>
       </c>
+      <c r="AA43" s="15">
+        <v>8</v>
+      </c>
+      <c r="AB43" s="15">
+        <v>8</v>
+      </c>
+      <c r="AC43" s="15">
+        <v>8</v>
+      </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:30">
+      <c r="A44" t="s">
         <v>58</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F43" t="s">
-        <v>60</v>
-      </c>
-      <c r="G43" t="s">
-        <v>60</v>
-      </c>
-      <c r="H43" t="s">
-        <v>60</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K43" t="s">
-        <v>60</v>
-      </c>
-      <c r="L43" t="s">
-        <v>60</v>
-      </c>
-      <c r="M43" t="s">
-        <v>60</v>
-      </c>
-      <c r="N43" t="s">
-        <v>60</v>
-      </c>
-      <c r="O43" t="s">
-        <v>60</v>
-      </c>
-      <c r="P43" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>60</v>
-      </c>
-      <c r="R43" t="s">
-        <v>60</v>
-      </c>
-      <c r="S43" t="s">
-        <v>60</v>
-      </c>
-      <c r="T43" t="s">
-        <v>60</v>
-      </c>
-      <c r="U43" t="s">
-        <v>60</v>
-      </c>
-      <c r="V43" t="s">
-        <v>60</v>
-      </c>
-      <c r="W43" t="s">
-        <v>60</v>
-      </c>
-      <c r="X43" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
       </c>
       <c r="E44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="H44" t="s">
-        <v>42</v>
-      </c>
-      <c r="I44" t="s">
-        <v>42</v>
-      </c>
-      <c r="J44" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="K44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="L44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="M44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="N44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="O44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="P44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="Q44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="R44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="S44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="T44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="U44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="V44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="W44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="X44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="Y44" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="Z44" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30">
       <c r="A45" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>20</v>
@@ -4418,79 +4898,88 @@
       <c r="C45" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D45" t="s">
-        <v>45</v>
+      <c r="D45" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="P45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="Q45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="R45" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="S45" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="T45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="U45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="V45" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="W45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="X45" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="Y45" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="Z45" t="s">
-        <v>113</v>
+        <v>42</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
+    <row r="46" spans="1:30">
+      <c r="A46" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>20</v>
@@ -4499,28 +4988,118 @@
         <v>36</v>
       </c>
       <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46" t="s">
+        <v>45</v>
+      </c>
+      <c r="J46" t="s">
+        <v>45</v>
+      </c>
+      <c r="K46" t="s">
+        <v>45</v>
+      </c>
+      <c r="L46" t="s">
+        <v>45</v>
+      </c>
+      <c r="M46" t="s">
+        <v>45</v>
+      </c>
+      <c r="N46" t="s">
+        <v>45</v>
+      </c>
+      <c r="O46" t="s">
+        <v>90</v>
+      </c>
+      <c r="P46" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>90</v>
+      </c>
+      <c r="R46" t="s">
+        <v>113</v>
+      </c>
+      <c r="S46" t="s">
+        <v>90</v>
+      </c>
+      <c r="T46" t="s">
+        <v>113</v>
+      </c>
+      <c r="U46" t="s">
+        <v>90</v>
+      </c>
+      <c r="V46" t="s">
+        <v>90</v>
+      </c>
+      <c r="W46" t="s">
+        <v>113</v>
+      </c>
+      <c r="X46" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
         <v>49</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K47" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:30">
+      <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automatic validation for csp added
</commit_message>
<xml_diff>
--- a/reskit/csp/data/CSP_database.xlsx
+++ b/reskit/csp/data/CSP_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\reskit\reskit\csp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DCE6A~1.FRA\DOCUME~1\MobaXterm\slash\RemoteFiles\67580_2_145\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4E13A3-CAF2-49E8-BAB4-BBFDC901E4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF8C1A2-6BBC-472D-B5DA-7743EB1B887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="138">
   <si>
     <t>Parameter</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>OPEX_perc_CAPEX</t>
+  </si>
+  <si>
+    <t>Dataset_Heliosol_2030_validation3</t>
   </si>
 </sst>
 </file>
@@ -936,32 +939,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
-  <dimension ref="A1:AD48"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="U39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="27.5546875" hidden="1" customWidth="1"/>
-    <col min="17" max="19" width="27.5546875" customWidth="1"/>
-    <col min="20" max="20" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="29" width="27.5546875" customWidth="1"/>
-    <col min="30" max="30" width="59.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="18" width="27.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="27.5703125" customWidth="1"/>
+    <col min="20" max="20" width="30.42578125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="27.5703125" hidden="1" customWidth="1"/>
+    <col min="22" max="30" width="27.5703125" customWidth="1"/>
+    <col min="31" max="31" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,31 +1033,34 @@
         <v>98</v>
       </c>
       <c r="W1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>101</v>
       </c>
       <c r="X2" s="15" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="Y2" s="15" t="s">
         <v>80</v>
@@ -1130,16 +1137,19 @@
         <v>80</v>
       </c>
       <c r="AA2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AC2" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AD2" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1207,7 +1217,7 @@
         <v>18</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>18</v>
@@ -1227,11 +1237,14 @@
       <c r="AC3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1319,11 +1332,14 @@
       <c r="AC4" s="16">
         <v>8.7266462599716496E-5</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="AE4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1411,11 +1427,14 @@
       <c r="AC5" s="16">
         <v>3.1070976818244299E-5</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="AE5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1503,11 +1522,14 @@
       <c r="AC6" s="15">
         <v>0</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1574,8 +1596,8 @@
       <c r="V7" s="15">
         <v>0.82699999999999996</v>
       </c>
-      <c r="W7" s="15">
-        <v>0.82699999999999996</v>
+      <c r="W7" s="13">
+        <v>0.92688000000000004</v>
       </c>
       <c r="X7" s="15">
         <v>0.82699999999999996</v>
@@ -1595,11 +1617,14 @@
       <c r="AC7" s="15">
         <v>0.82699999999999996</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="15">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AE7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1658,8 +1683,11 @@
       <c r="AC8" s="15">
         <v>-1</v>
       </c>
+      <c r="AD8" s="15">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1747,11 +1775,14 @@
       <c r="AC9" s="15">
         <v>16</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="15">
+        <v>16</v>
+      </c>
+      <c r="AE9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1839,11 +1870,14 @@
       <c r="AC10" s="15">
         <v>0</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AD10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +1948,7 @@
         <v>4.4701935910452802E-2</v>
       </c>
       <c r="X11" s="15">
-        <v>4.4701935910452829E-2</v>
+        <v>4.4701935910452802E-2</v>
       </c>
       <c r="Y11" s="15">
         <v>4.4701935910452829E-2</v>
@@ -1923,19 +1957,22 @@
         <v>4.4701935910452829E-2</v>
       </c>
       <c r="AA11" s="15">
+        <v>4.4701935910452829E-2</v>
+      </c>
+      <c r="AB11" s="15">
         <v>4.4701935910452802E-2</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AC11" s="15">
         <v>4.4701935910452829E-2</v>
       </c>
-      <c r="AC11" s="15">
+      <c r="AD11" s="15">
         <v>4.4701935910452802E-2</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2023,11 +2060,14 @@
       <c r="AC12" s="15">
         <v>-2.9278818932777496E-4</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="AE12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2115,11 +2155,14 @@
       <c r="AC13" s="15">
         <v>1.2085236947426394E-6</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AD13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="AE13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2207,11 +2250,14 @@
       <c r="AC14" s="15">
         <v>-4.6531969642924003E-10</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="AE14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2297,8 +2343,11 @@
       <c r="AC15" s="15" t="s">
         <v>99</v>
       </c>
+      <c r="AD15" s="15" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -2384,8 +2433,11 @@
       <c r="AC16" s="15">
         <v>0.38</v>
       </c>
+      <c r="AD16" s="15">
+        <v>0.38</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -2471,8 +2523,11 @@
       <c r="AC17" s="15">
         <v>0.3</v>
       </c>
+      <c r="AD17" s="15">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2561,8 +2616,11 @@
       <c r="AC18" s="10">
         <v>-1</v>
       </c>
+      <c r="AD18" s="10">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2650,11 +2708,14 @@
       <c r="AC19" s="15">
         <v>0.96</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AD19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="AE19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -2742,8 +2803,11 @@
       <c r="AC20" s="15">
         <v>0.99</v>
       </c>
+      <c r="AD20" s="15">
+        <v>0.99</v>
+      </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2831,11 +2895,14 @@
       <c r="AC21">
         <v>0.108</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AD21">
+        <v>0.108</v>
+      </c>
+      <c r="AE21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2923,11 +2990,14 @@
       <c r="AC22" s="16">
         <v>0</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AD22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3015,11 +3085,14 @@
       <c r="AC23" s="15">
         <v>830</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AD23" s="15">
+        <v>830</v>
+      </c>
+      <c r="AE23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3107,11 +3180,14 @@
       <c r="AC24" s="7">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AD24" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AE24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3199,11 +3275,14 @@
       <c r="AC25" s="7">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AD25" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AE25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -3291,11 +3370,14 @@
       <c r="AC26" s="7">
         <v>0.05</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AD26" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AE26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -3383,11 +3465,14 @@
       <c r="AC27" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AD27" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AE27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3475,11 +3560,14 @@
       <c r="AC28" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AD28" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AE28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -3547,31 +3635,34 @@
         <v>6500</v>
       </c>
       <c r="W29" s="7">
+        <v>3100</v>
+      </c>
+      <c r="X29" s="7">
         <v>2634.2857142857142</v>
-      </c>
-      <c r="X29" s="19">
-        <v>3688</v>
       </c>
       <c r="Y29" s="19">
         <v>3688</v>
       </c>
-      <c r="Z29" s="7">
+      <c r="Z29" s="19">
+        <v>3688</v>
+      </c>
+      <c r="AA29" s="7">
         <v>6500</v>
       </c>
-      <c r="AA29" s="7">
+      <c r="AB29" s="7">
         <v>2634.2857142857142</v>
       </c>
-      <c r="AB29" s="7">
+      <c r="AC29" s="7">
         <v>6500</v>
       </c>
-      <c r="AC29" s="7">
+      <c r="AD29" s="7">
         <v>2634.2857142857142</v>
       </c>
-      <c r="AD29" t="s">
+      <c r="AE29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -3615,25 +3706,28 @@
         <v>0.39100000000000001</v>
       </c>
       <c r="X30" s="7">
-        <v>0.38400000000000001</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="Y30" s="7">
         <v>0.38400000000000001</v>
       </c>
       <c r="Z30" s="7">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="AA30" s="7">
         <v>0.42699999999999999</v>
       </c>
-      <c r="AA30" s="7">
+      <c r="AB30" s="7">
         <v>0.39100000000000001</v>
       </c>
-      <c r="AB30" s="7">
+      <c r="AC30" s="7">
         <v>0.42699999999999999</v>
       </c>
-      <c r="AC30" s="7">
+      <c r="AD30" s="7">
         <v>0.39100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -3721,8 +3815,11 @@
       <c r="AC31">
         <v>0.98</v>
       </c>
+      <c r="AD31">
+        <v>0.98</v>
+      </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -3792,29 +3889,32 @@
       <c r="W32" s="15">
         <v>405</v>
       </c>
-      <c r="X32" s="7">
-        <v>385</v>
+      <c r="X32" s="15">
+        <v>405</v>
       </c>
       <c r="Y32" s="7">
         <v>385</v>
       </c>
       <c r="Z32" s="7">
+        <v>385</v>
+      </c>
+      <c r="AA32" s="7">
         <v>560</v>
       </c>
-      <c r="AA32" s="15">
+      <c r="AB32" s="15">
         <v>405</v>
       </c>
-      <c r="AB32" s="7">
+      <c r="AC32" s="7">
         <v>560</v>
       </c>
-      <c r="AC32" s="15">
+      <c r="AD32" s="15">
         <v>405</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AE32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3884,29 +3984,32 @@
       <c r="W33" s="15">
         <v>-20</v>
       </c>
-      <c r="X33" s="7">
-        <v>60</v>
+      <c r="X33" s="15">
+        <v>-20</v>
       </c>
       <c r="Y33" s="7">
         <v>60</v>
       </c>
       <c r="Z33" s="7">
+        <v>60</v>
+      </c>
+      <c r="AA33" s="7">
         <v>260</v>
       </c>
-      <c r="AA33" s="15">
+      <c r="AB33" s="15">
         <v>-20</v>
       </c>
-      <c r="AB33" s="7">
+      <c r="AC33" s="7">
         <v>260</v>
       </c>
-      <c r="AC33" s="15">
+      <c r="AD33" s="15">
         <v>-20</v>
       </c>
-      <c r="AD33" t="s">
+      <c r="AE33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -3976,7 +4079,7 @@
       <c r="W34" s="15">
         <v>290</v>
       </c>
-      <c r="X34" s="7">
+      <c r="X34" s="15">
         <v>290</v>
       </c>
       <c r="Y34" s="7">
@@ -3985,20 +4088,23 @@
       <c r="Z34" s="7">
         <v>290</v>
       </c>
-      <c r="AA34" s="15">
+      <c r="AA34" s="7">
         <v>290</v>
       </c>
-      <c r="AB34" s="7">
+      <c r="AB34" s="15">
         <v>290</v>
       </c>
-      <c r="AC34" s="15">
+      <c r="AC34" s="7">
         <v>290</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AD34" s="15">
+        <v>290</v>
+      </c>
+      <c r="AE34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -4086,8 +4192,11 @@
       <c r="AC35">
         <v>25</v>
       </c>
+      <c r="AD35">
+        <v>25</v>
+      </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -4158,25 +4267,28 @@
         <v>1003.2</v>
       </c>
       <c r="X36" s="15">
+        <v>1003.2</v>
+      </c>
+      <c r="Y36" s="15">
         <v>1056</v>
       </c>
-      <c r="Y36" s="15">
+      <c r="Z36" s="15">
         <v>1003.2</v>
-      </c>
-      <c r="Z36" s="15">
-        <v>922.94399999999996</v>
       </c>
       <c r="AA36" s="15">
         <v>922.94399999999996</v>
       </c>
       <c r="AB36" s="15">
-        <v>882.81600000000003</v>
+        <v>922.94399999999996</v>
       </c>
       <c r="AC36" s="15">
         <v>882.81600000000003</v>
       </c>
+      <c r="AD36" s="15">
+        <v>882.81600000000003</v>
+      </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -4246,26 +4358,29 @@
       <c r="W37" s="15">
         <v>36.96</v>
       </c>
-      <c r="X37" s="7">
+      <c r="X37" s="15">
+        <v>36.96</v>
+      </c>
+      <c r="Y37" s="7">
         <v>44</v>
       </c>
-      <c r="Y37" s="7">
+      <c r="Z37" s="7">
         <v>36.96</v>
       </c>
-      <c r="Z37" s="7">
+      <c r="AA37" s="7">
         <v>23.478400000000001</v>
       </c>
-      <c r="AA37" s="15">
+      <c r="AB37" s="15">
         <v>34.0032</v>
       </c>
-      <c r="AB37" s="7">
+      <c r="AC37" s="7">
         <v>22.457599999999999</v>
       </c>
-      <c r="AC37" s="15">
+      <c r="AD37" s="15">
         <v>32.524799999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -4335,26 +4450,29 @@
       <c r="W38" s="15">
         <v>192.72</v>
       </c>
-      <c r="X38" s="7">
+      <c r="X38" s="15">
+        <v>192.72</v>
+      </c>
+      <c r="Y38" s="7">
         <v>220</v>
       </c>
-      <c r="Y38" s="7">
+      <c r="Z38" s="7">
         <v>172.21600000000001</v>
       </c>
-      <c r="Z38" s="7">
+      <c r="AA38" s="7">
         <v>152.19999999999999</v>
       </c>
-      <c r="AA38" s="15">
+      <c r="AB38" s="15">
         <v>177.30240000000001</v>
       </c>
-      <c r="AB38" s="7">
+      <c r="AC38" s="7">
         <v>145.5872</v>
       </c>
-      <c r="AC38" s="15">
+      <c r="AD38" s="15">
         <v>169.59360000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -4424,26 +4542,29 @@
       <c r="W39" s="15">
         <v>0.88</v>
       </c>
-      <c r="X39" s="7">
+      <c r="X39" s="15">
         <v>0.88</v>
       </c>
       <c r="Y39" s="7">
         <v>0.88</v>
       </c>
       <c r="Z39" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="AA39" s="7">
         <v>0.8196</v>
       </c>
-      <c r="AA39" s="15">
+      <c r="AB39" s="15">
         <v>0.8196</v>
       </c>
-      <c r="AB39" s="7">
+      <c r="AC39" s="7">
         <v>0.77439999999999998</v>
       </c>
-      <c r="AC39" s="15">
+      <c r="AD39" s="15">
         <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -4513,26 +4634,29 @@
       <c r="W40" s="15">
         <v>11</v>
       </c>
-      <c r="X40" s="7">
+      <c r="X40" s="15">
+        <v>11</v>
+      </c>
+      <c r="Y40" s="7">
         <v>15</v>
-      </c>
-      <c r="Y40" s="7">
-        <v>11</v>
       </c>
       <c r="Z40" s="7">
         <v>11</v>
       </c>
-      <c r="AA40" s="15">
+      <c r="AA40" s="7">
         <v>11</v>
       </c>
-      <c r="AB40" s="7">
+      <c r="AB40" s="15">
         <v>11</v>
       </c>
-      <c r="AC40" s="15">
+      <c r="AC40" s="7">
         <v>11</v>
       </c>
+      <c r="AD40" s="15">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -4602,7 +4726,7 @@
       <c r="W41" s="15">
         <v>2</v>
       </c>
-      <c r="X41" s="7">
+      <c r="X41" s="15">
         <v>2</v>
       </c>
       <c r="Y41" s="7">
@@ -4611,17 +4735,20 @@
       <c r="Z41" s="7">
         <v>2</v>
       </c>
-      <c r="AA41" s="15">
+      <c r="AA41" s="7">
         <v>2</v>
       </c>
-      <c r="AB41" s="7">
+      <c r="AB41" s="15">
         <v>2</v>
       </c>
-      <c r="AC41" s="15">
+      <c r="AC41" s="7">
         <v>2</v>
       </c>
+      <c r="AD41" s="15">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -4709,8 +4836,11 @@
       <c r="AC42" s="15">
         <v>0.05</v>
       </c>
+      <c r="AD42" s="15">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -4798,8 +4928,11 @@
       <c r="AC43" s="15">
         <v>8</v>
       </c>
+      <c r="AD43" s="15">
+        <v>8</v>
+      </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -4887,8 +5020,11 @@
       <c r="AC44" t="s">
         <v>60</v>
       </c>
+      <c r="AD44" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:31">
       <c r="A45" s="3" t="s">
         <v>32</v>
       </c>
@@ -4976,8 +5112,11 @@
       <c r="AC45" t="s">
         <v>42</v>
       </c>
+      <c r="AD45" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:31">
       <c r="A46" s="3" t="s">
         <v>35</v>
       </c>
@@ -5048,25 +5187,28 @@
         <v>111</v>
       </c>
       <c r="X46" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="Y46" t="s">
         <v>133</v>
       </c>
       <c r="Z46" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA46" t="s">
         <v>90</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AB46" t="s">
         <v>111</v>
       </c>
-      <c r="AB46" t="s">
+      <c r="AC46" t="s">
         <v>90</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AD46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -5083,7 +5225,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
         <v>72</v>
       </c>

</xml_diff>